<commit_message>
Fixed solution xls for ex2.
</commit_message>
<xml_diff>
--- a/Fundementals/Solution/BikeStoreSample.xlsx
+++ b/Fundementals/Solution/BikeStoreSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Elevation\Excel\Fundementals\Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4FC26A-0248-444C-9A9F-AA4FC8F3739B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FF715D-3259-4E5E-A9CF-37F421A2BDBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2655" windowWidth="30120" windowHeight="11385" activeTab="1" xr2:uid="{E731B28F-D92B-4ABF-AE71-A2BC403318D1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E731B28F-D92B-4ABF-AE71-A2BC403318D1}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderDetailsData" sheetId="1" r:id="rId1"/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4CAE42-8427-4763-99BF-87F494943F45}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7146,11 +7146,17 @@
         <f>COUNTIF(B2:B100,1)</f>
         <v>35</v>
       </c>
-      <c r="B101" s="2"/>
+      <c r="B101" s="2">
+        <f>COUNT(B2:B100)</f>
+        <v>99</v>
+      </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="9"/>
+      <c r="F101" s="9">
+        <f>AVERAGE(F2:F100)</f>
+        <v>1396.3851515151528</v>
+      </c>
       <c r="G101" s="2">
         <f>SUM(G2:G100)</f>
         <v>146</v>
@@ -7161,8 +7167,8 @@
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="9">
-        <f>SUM(J2:J100)</f>
-        <v>16399.289899999989</v>
+        <f>AVERAGE(J2:J100)</f>
+        <v>165.64939292929282</v>
       </c>
       <c r="K101" s="11">
         <f>SUM(K2:K100)</f>
@@ -7183,7 +7189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0669B-A8EB-4D1F-8021-CE894C392FA0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test for ex3 countif/sumif functions. (Column A).
</commit_message>
<xml_diff>
--- a/Fundementals/Solution/BikeStoreSample.xlsx
+++ b/Fundementals/Solution/BikeStoreSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Elevation\Excel\Fundementals\Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FF715D-3259-4E5E-A9CF-37F421A2BDBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AED76F-78B9-41AE-BB8A-1E73AAC1F2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E731B28F-D92B-4ABF-AE71-A2BC403318D1}"/>
   </bookViews>
@@ -923,7 +923,7 @@
   <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>